<commit_message>
add new in presentation, add subgraphs colors
</commit_message>
<xml_diff>
--- a/Результаты в экселях/Subgrapsh_unification.xlsx
+++ b/Результаты в экселях/Subgrapsh_unification.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1185" windowWidth="21570" windowHeight="11325" activeTab="5"/>
+    <workbookView minimized="1" xWindow="1125" yWindow="1185" windowWidth="21570" windowHeight="11325" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Общая выборка" sheetId="11" r:id="rId1"/>
@@ -18,6 +18,8 @@
     <sheet name="Сумма" sheetId="14" r:id="rId4"/>
     <sheet name="Общая выборка уровень знач 0.1" sheetId="15" r:id="rId5"/>
     <sheet name="Робастный метод" sheetId="16" r:id="rId6"/>
+    <sheet name="Лист1" sheetId="17" r:id="rId7"/>
+    <sheet name="Лист2" sheetId="18" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="503" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="545" uniqueCount="292">
   <si>
     <t>short_101.A@OD1_79.A@NH2_101.A@OD2_79.A@NH1_81.A@O_74.A@O_83.A@O</t>
   </si>
@@ -863,13 +865,61 @@
   </si>
   <si>
     <t>x9            -1.3295      0.449     -2.961      0.003      -2.209      -0.450</t>
+  </si>
+  <si>
+    <t>Оценки</t>
+  </si>
+  <si>
+    <t>rmse: 3.865618748066464</t>
+  </si>
+  <si>
+    <t>rmse: 3.788002757687708</t>
+  </si>
+  <si>
+    <t>x1</t>
+  </si>
+  <si>
+    <t>x2</t>
+  </si>
+  <si>
+    <t>x3</t>
+  </si>
+  <si>
+    <t>x4</t>
+  </si>
+  <si>
+    <t>x5</t>
+  </si>
+  <si>
+    <t>x6</t>
+  </si>
+  <si>
+    <t>x7</t>
+  </si>
+  <si>
+    <t>x8</t>
+  </si>
+  <si>
+    <t>x9</t>
+  </si>
+  <si>
+    <t>Ordinary</t>
+  </si>
+  <si>
+    <t>Robust</t>
+  </si>
+  <si>
+    <t>n значений валидаций</t>
+  </si>
+  <si>
+    <t>RMSE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -930,6 +980,15 @@
     <font>
       <sz val="18"/>
       <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -1009,13 +1068,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
@@ -1025,14 +1085,19 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="4"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
+    <cellStyle name="Гиперссылка" xfId="4" builtinId="8"/>
     <cellStyle name="Нейтральный" xfId="3" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="2" builtinId="27"/>
@@ -1214,14 +1279,14 @@
     <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>662543</xdr:colOff>
-      <xdr:row>94</xdr:row>
-      <xdr:rowOff>69272</xdr:rowOff>
+      <xdr:row>98</xdr:row>
+      <xdr:rowOff>209345</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>53039</xdr:colOff>
-      <xdr:row>111</xdr:row>
-      <xdr:rowOff>173181</xdr:rowOff>
+      <xdr:row>116</xdr:row>
+      <xdr:rowOff>117152</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1238,8 +1303,89 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6204361" y="19794681"/>
-          <a:ext cx="10768542" cy="3671455"/>
+          <a:off x="6153425" y="19665558"/>
+          <a:ext cx="10736452" cy="3479682"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>22578</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>95877</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Рисунок 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="13232072" cy="4496427"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>294409</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>51954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>39</xdr:col>
+      <xdr:colOff>499510</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>14647</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Рисунок 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="15534409" y="51954"/>
+          <a:ext cx="12419367" cy="4119057"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1551,7 +1697,7 @@
   <dimension ref="A1:Z73"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U16" sqref="U16"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1560,34 +1706,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="9" t="s">
         <v>7</v>
       </c>
       <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="9" t="s">
         <v>9</v>
       </c>
       <c r="O1" t="s">
@@ -3997,8 +4143,19 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1"/>
+    <hyperlink ref="B1" r:id="rId2"/>
+    <hyperlink ref="C1" r:id="rId3"/>
+    <hyperlink ref="D1" r:id="rId4"/>
+    <hyperlink ref="E1" r:id="rId5"/>
+    <hyperlink ref="F1" r:id="rId6"/>
+    <hyperlink ref="G1" r:id="rId7"/>
+    <hyperlink ref="H1" r:id="rId8"/>
+    <hyperlink ref="J1" r:id="rId9"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId10"/>
 </worksheet>
 </file>
 
@@ -10022,10 +10179,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y121"/>
+  <dimension ref="A1:Y125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="F65" sqref="F65"/>
+    <sheetView topLeftCell="B21" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="V36" sqref="V36:Y38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10242,7 +10399,7 @@
       <c r="A37" t="s">
         <v>113</v>
       </c>
-      <c r="V37" s="9" t="s">
+      <c r="V37" s="10" t="s">
         <v>258</v>
       </c>
       <c r="W37" s="7">
@@ -10259,7 +10416,7 @@
       <c r="A38" t="s">
         <v>114</v>
       </c>
-      <c r="V38" s="10"/>
+      <c r="V38" s="11"/>
       <c r="W38" s="7">
         <v>0.51500000000000001</v>
       </c>
@@ -10547,136 +10704,146 @@
         <v>11</v>
       </c>
     </row>
-    <row r="97" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A97" s="6" t="s">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="99" spans="1:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A99" s="6" t="s">
         <v>233</v>
       </c>
-      <c r="B97" s="6"/>
-      <c r="C97" s="6"/>
-      <c r="D97" s="6"/>
-      <c r="E97" s="6"/>
-      <c r="F97" s="6"/>
-      <c r="G97" s="6"/>
-      <c r="H97" s="6"/>
-    </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
-        <v>234</v>
-      </c>
+      <c r="B99" s="6"/>
+      <c r="C99" s="6"/>
+      <c r="D99" s="6"/>
+      <c r="E99" s="6"/>
+      <c r="F99" s="6"/>
+      <c r="G99" s="6"/>
+      <c r="H99" s="6"/>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>262</v>
+        <v>11</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>263</v>
+        <v>234</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>235</v>
+        <v>262</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>236</v>
+        <v>263</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>264</v>
+        <v>237</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>265</v>
+        <v>238</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>11</v>
+        <v>264</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>239</v>
+        <v>265</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>266</v>
+        <v>239</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>267</v>
+        <v>22</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A122" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A123" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A125" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -10687,4 +10854,342 @@
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I23"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13:E23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I2" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="I4" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+      <c r="I6" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I7" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="I9" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I10" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>32</v>
+      </c>
+      <c r="I11" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="E13" s="7" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C14" s="7" t="s">
+        <v>279</v>
+      </c>
+      <c r="D14" s="7">
+        <v>1.17</v>
+      </c>
+      <c r="E14" s="7">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C15" s="7" t="s">
+        <v>280</v>
+      </c>
+      <c r="D15" s="7">
+        <v>-14.49</v>
+      </c>
+      <c r="E15" s="7">
+        <v>-13.56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="C16" s="7" t="s">
+        <v>281</v>
+      </c>
+      <c r="D16" s="7">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="E16" s="7">
+        <v>9.61</v>
+      </c>
+    </row>
+    <row r="17" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C17" s="7" t="s">
+        <v>282</v>
+      </c>
+      <c r="D17" s="7">
+        <v>1.76</v>
+      </c>
+      <c r="E17" s="7">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="18" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C18" s="7" t="s">
+        <v>283</v>
+      </c>
+      <c r="D18" s="7">
+        <v>7.91</v>
+      </c>
+      <c r="E18" s="7">
+        <v>7.53</v>
+      </c>
+    </row>
+    <row r="19" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C19" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="D19" s="7">
+        <v>1.6</v>
+      </c>
+      <c r="E19" s="7">
+        <v>1.71</v>
+      </c>
+    </row>
+    <row r="20" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C20" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="D20" s="7">
+        <v>1.71</v>
+      </c>
+      <c r="E20" s="7">
+        <v>1.79</v>
+      </c>
+    </row>
+    <row r="21" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="D21" s="7">
+        <v>6.08</v>
+      </c>
+      <c r="E21" s="7">
+        <v>5.8</v>
+      </c>
+    </row>
+    <row r="22" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C22" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="D22" s="7">
+        <v>-1.56</v>
+      </c>
+      <c r="E22" s="7">
+        <v>-1.32</v>
+      </c>
+    </row>
+    <row r="23" spans="3:5" x14ac:dyDescent="0.25">
+      <c r="C23" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23" s="7">
+        <v>4.93</v>
+      </c>
+      <c r="E23" s="7">
+        <v>4.28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A22:X37"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I36" sqref="I36:K37"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="10" max="10" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="23.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="14" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="X22">
+        <v>11.7864542772553</v>
+      </c>
+    </row>
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>11.4812028033598</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T28" s="7"/>
+      <c r="U28" s="7" t="s">
+        <v>290</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T29" s="12" t="s">
+        <v>258</v>
+      </c>
+      <c r="U29" s="7">
+        <v>1</v>
+      </c>
+      <c r="V29" s="7">
+        <v>11.4812028033598</v>
+      </c>
+      <c r="W29" s="7">
+        <v>11.7864542772553</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T30" s="12"/>
+      <c r="U30" s="7">
+        <v>6</v>
+      </c>
+      <c r="V30" s="7">
+        <v>11.9174878852891</v>
+      </c>
+      <c r="W30" s="7">
+        <v>13.0680419189116</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T31" s="12"/>
+      <c r="U31" s="7">
+        <v>9</v>
+      </c>
+      <c r="V31" s="7">
+        <v>10.039131339009501</v>
+      </c>
+      <c r="W31" s="7">
+        <v>11.076645415337699</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="T32" s="12"/>
+      <c r="U32" s="7">
+        <v>12</v>
+      </c>
+      <c r="V32" s="7">
+        <v>11.2382080090554</v>
+      </c>
+      <c r="W32" s="7">
+        <v>12.380488624875399</v>
+      </c>
+    </row>
+    <row r="36" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I36" s="7"/>
+      <c r="J36" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="K36" s="7" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="37" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I37" s="7" t="s">
+        <v>291</v>
+      </c>
+      <c r="J37" s="7">
+        <v>3.7880027576876998</v>
+      </c>
+      <c r="K37" s="7">
+        <v>3.8656187480664599</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="T29:T32"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>